<commit_message>
feature engineering e ajustando coleta de dados vagas.com
</commit_message>
<xml_diff>
--- a/data/data_raw/tmp/data_csv/cientista_de_dados_vagas.xlsx
+++ b/data/data_raw/tmp/data_csv/cientista_de_dados_vagas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,15 +511,20 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>pcd</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>beneficios</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>codigo_vaga</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>descricao</t>
         </is>
@@ -549,7 +554,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-02-03</t>
+          <t>2024-02-07</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -583,27 +588,24 @@
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Não informado</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>Regime CLT</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>['Assistência médica', 'Assistência odontológica', 'Seguro de vida', 'Vale-alimentação', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>v2600201</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>Descrição
 Descrição: Principais responsabilidades:
@@ -647,19 +649,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.vagas.com.br/vagas/v2599448/especialista-em-engenharia-de-dados</t>
+          <t>https://www.vagas.com.br/vagas/v2608824/cientista-de-dados-senior</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Publicada em 08/01/2024</t>
+          <t>Publicada há 2 dias</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-02-03</t>
+          <t>2024-02-07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -674,12 +676,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Especialista em Engenharia de Dados</t>
+          <t>Cientista de Dados Sênior</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Recovery</t>
+          <t>TOTVS</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -689,11 +691,7 @@
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Não informado</t>
-        </is>
-      </c>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
           <t>Regime CLT</t>
@@ -702,13 +700,33 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>v2599448</t>
+          <t>['Assistência médica', 'Assistência odontológica', 'Auxílio creche', 'Bicicletário', 'Convênio com empresas parceiras', 'Participação nos Lucros ou Resultados', 'Previdência privada', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
+          <t>v2608824</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
           <t>Descrição
-Descrição: Na Recovery o(a) Especialista de Engenharia de Dados tem a missão de desenvolver e manter a nossa plataforma de dados estável e performática, além de aplicar técnicas de análise e modelagem para gerar insights. Garantir a qualidade, integridade e segurança dos dados, assim como colaborar de forma interdisciplinar com outros times, incluindo cientista de dados, engenheiro de softwares, analista de processos, entre outros, a fim de entender a dor do cliente e propor soluções e/ou melhorias nos processos.Todas as vagas publicadas são abertas para pessoas com deficiência. A Recovery é uma empresa que valoriza a diversidade e está em busca da construção de um ambiente mais inclusivo. Aqui todos os candidatos são bem-vindos!O que seria bacana você ter:•	Graduação completa na área de tecnologia (ciência da computação, sistemas de informação ou áreas correlatas);•	Experiência na área de Engenharia de Dados;•	Experiência em Azure Data Factory, Airflow e SSIS (integration services);•	Experiência em bancos SQL e NoSQL;•	Conhecimentos avançados em SQL, Python, Spark e PySpark;•	Experiência em Databricks;•	Conhecimentos em soluções de Engenharia de Dados em nuvem (Azure e AWS);•	Experiência em arquiteturas Data Lake e Lakehouse;•	Conhecimentos em versionamento com Git;•	Comunicação clara e objetiva;•	Prática em documentação de processos.O que você terá que fazer: •	Migrar pipelines para a nova plataforma de dados, revisando por completo o código e as regras de negócio;•	Construir novas pipelines de dados para coletar, processar e armazenar dados no Lakehouse, garantido a qualidade das informações;•	Avaliar periodicamente o desempenho das soluções de dados construídas e identificar oportunidades de melhorias;•	Apoiar na definição de arquitetura de solução de dados;•	Ser referência técnica para o time;•	Desenvolver bibliotecas e frameworks para auxiliar na padronização, segurança e performance dos processos;•	Entender o business de cada cliente, bem como suas dores, a fim de propor soluções de dados, propor melhorias nos processos e melhorar a sua experiência como usuário da plataforma de dados;•	Conduzir reuniões com os stakeholders;•	Promover a cultura data driven para todos os times.Para fechar com chave de ouro, será considerado um diferencial:•	Ter atuado em projeto de migração de DW para ambientes Data Lake ou Lakehouse;•	Conhecimento em soluções de observabilidade para monitoramento dos processos;•	Ter atuado com framework Scrum.O que oferecemos de principais benefícios para os nossos Reclovers: •	Vale Alimentação ou refeição no valor de R$ 1000 por mês, inclusive no mês das suas férias;•	Assistência médica e odontológica estendida aos dependentes; •	Participação nos Lucros e Resultados; •	Seguro de vida.Quer saber o que mais temos de legal por aqui? Dá uma olhada!•	Estimulamos que o nosso time esteja sempre em movimento, para isso temos por aqui o GymPass;•	Day off no mês do seu aniversário e sorteio de vale presente para os aniversariantes do mês;•	Nas sextas-feiras o nosso o expediente se encerra as 16h #Sextou;•	Vestimenta Casual (todos os dias): aqui você pode ser quem é! ;)•	Disponibilizamos frutas no escritório;•	Por aqui gostamos de celebrar os bons momentos, por isso temos Happy Hour com a galera no escritório 1x no mês com chopp e comidinhas;•	Auxílio Home Office de R$ 200,00 – Disponibilizado uma única vez;•	Auxílio Internet de R$ 100,00 – Disponibilizado mensalmente;•	Somos uma empresa cidadã! Licença maternidade e paternidade estendida para nossos Reclovers: 6 meses para mamães e 20 dias para os papais;•	Auxílio-creche para as mamães;•	Fique OK – Programa de apoio social para orientações através de profissionais como: psicólogo, assistente social, advogado, nutricionista, consultor financeiro, consultor pet, fisioterapeuta e personal trainer;•	Estamos trabalhando em modelo híbrido e nosso escritório fica no coração de São Paulo, a Avenida Paulista!Quer ser parte do nosso time? Vem, #todosjuntos fazemos a diferença!</t>
+Descrição: Acreditamos no poder transformador da tecnologia e na sua capacidade de contribuir para a construção de uma sociedade mais diversa e inclusiva. Como a maior empresa brasileira de tecnologia, temos o compromisso com uma política e programa de diversidade e inclusão para termos um ecossistema cada vez mais representativo, respeitoso e acolhedor.O QUE VOCÊ VAI FAZER:
+Analisar dados da carteira de clientes, buscando a identificação e segmentação nos diferentes perfis;
+Desenvolver modelos preditivos com base nos comportamentos;
+Tratar os dados existentes ou externos para produzir conhecimento que possa subsidiar a tomada de decisões;
+Realizar estudos estatísticos por análises de dados avançados para criar hipóteses para fidelizar, reter e conquistar mais clientes;
+Elaborar apresentações para explorar e expor os resultados dos modelos e descobertas;
+Desenvolver hipóteses por análise de dados avançados;
+Tratamento, limpeza e exploração de dados;
+Qualificar os dados;
+Criar Dash com ferramentas de Mercado sobre estudo de nossos clientes;
+Apoiar na evolução de nossos painéis já criados.
+Outros requisitos: O QUE ESPERAMOS DE VOCÊ: 
+Linguagens de programação como Python, R, SQL e Java entre outros.
+Conhecimento de técnicas de análise de dados, como estatística, aprendizado de máquina e inteligência artificial.
+Atuação com Zendesk.
+INFORMAÇÕES ADICIONAIS:Oportunidade para atuar 2 dias presenciais na TOTVS Matriz - SP.</t>
         </is>
       </c>
     </row>
@@ -720,77 +738,218 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.vagas.com.br/vagas/v2600553/jovem-aprendiz-ti</t>
+          <t>https://www.vagas.com.br/vagas/v2609333/pessoa-cientista-de-aplicacao-tecnica-biologia</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Publicada ontem</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Cientista de Dados</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Pleno</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Pessoa Cientista de Aplicação Técnica (Biologia)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>METARH +humana</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Regime CLT</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>['Assistência médica', 'Assistência odontológica', 'Vale-refeição', 'Vale-transporte']</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>v2609333</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Descrição
+Descrição: •	Será responsável por fornecer orientação técnica e suporte aos nossos clientes de “Sequenciamento de Próxima Geração” em questões técnicas e relacionadas a serviços, além de demonstrar usos e vantagens de nossos produtos•	A função é altamente multifuncional e trabalha em estreita colaboração com nossos engenheiros de serviço de campo, cientistas de aplicação de campo e com nossas equipes de vendas e marketing;•	Triagem profissional, eficiente e conclusiva, soluciona problemas e resolve as questões técnicas do cliente;•	Auxiliar os clientes com o projeto e a interpretação de experimentos e análises de sequenciamento de próxima geração; Fornecer orientação técnica sobre a escolha e uso do produto apropriado para clientes existentes e potenciais;•	Problemas de triagem e despacho que exigem suporte de campo para engenheiros e cientistas de aplicações da empresa;•	Registre e gerencie problemas de clientes usando o banco de dados de rastreamento de problemas.Idiomas:Inglês - Nível Fluente e Inglês - Nível AvançadoOutros requisitos: - Experiência laboratorial relevante em biologia molecular, genética, bioinformática ou áreas afins;- Inglês fluente;- Superior completo em Biologia ou áreas correlatas;- Desejável mestrado/ doutorado.Outras Informações: Local de Trabalho: bairro Cerqueira César - São Paulo - SP (atividade presencial)Modalidade de contratação: CLT - Terceirizado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Vagas.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.vagas.com.br/vagas/v2599448/especialista-em-engenharia-de-dados</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Publicada em 08/01/2024</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Cientista de Dados</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Sênior</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Especialista em Engenharia de Dados</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Recovery</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Regime CLT</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>v2599448</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Descrição
+Descrição: Na Recovery o(a) Especialista de Engenharia de Dados tem a missão de desenvolver e manter a nossa plataforma de dados estável e performática, além de aplicar técnicas de análise e modelagem para gerar insights. Garantir a qualidade, integridade e segurança dos dados, assim como colaborar de forma interdisciplinar com outros times, incluindo cientista de dados, engenheiro de softwares, analista de processos, entre outros, a fim de entender a dor do cliente e propor soluções e/ou melhorias nos processos.Todas as vagas publicadas são abertas para pessoas com deficiência. A Recovery é uma empresa que valoriza a diversidade e está em busca da construção de um ambiente mais inclusivo. Aqui todos os candidatos são bem-vindos!O que seria bacana você ter:•	Graduação completa na área de tecnologia (ciência da computação, sistemas de informação ou áreas correlatas);•	Experiência na área de Engenharia de Dados;•	Experiência em Azure Data Factory, Airflow e SSIS (integration services);•	Experiência em bancos SQL e NoSQL;•	Conhecimentos avançados em SQL, Python, Spark e PySpark;•	Experiência em Databricks;•	Conhecimentos em soluções de Engenharia de Dados em nuvem (Azure e AWS);•	Experiência em arquiteturas Data Lake e Lakehouse;•	Conhecimentos em versionamento com Git;•	Comunicação clara e objetiva;•	Prática em documentação de processos.O que você terá que fazer: •	Migrar pipelines para a nova plataforma de dados, revisando por completo o código e as regras de negócio;•	Construir novas pipelines de dados para coletar, processar e armazenar dados no Lakehouse, garantido a qualidade das informações;•	Avaliar periodicamente o desempenho das soluções de dados construídas e identificar oportunidades de melhorias;•	Apoiar na definição de arquitetura de solução de dados;•	Ser referência técnica para o time;•	Desenvolver bibliotecas e frameworks para auxiliar na padronização, segurança e performance dos processos;•	Entender o business de cada cliente, bem como suas dores, a fim de propor soluções de dados, propor melhorias nos processos e melhorar a sua experiência como usuário da plataforma de dados;•	Conduzir reuniões com os stakeholders;•	Promover a cultura data driven para todos os times.Para fechar com chave de ouro, será considerado um diferencial:•	Ter atuado em projeto de migração de DW para ambientes Data Lake ou Lakehouse;•	Conhecimento em soluções de observabilidade para monitoramento dos processos;•	Ter atuado com framework Scrum.O que oferecemos de principais benefícios para os nossos Reclovers: •	Vale Alimentação ou refeição no valor de R$ 1000 por mês, inclusive no mês das suas férias;•	Assistência médica e odontológica estendida aos dependentes; •	Participação nos Lucros e Resultados; •	Seguro de vida.Quer saber o que mais temos de legal por aqui? Dá uma olhada!•	Estimulamos que o nosso time esteja sempre em movimento, para isso temos por aqui o GymPass;•	Day off no mês do seu aniversário e sorteio de vale presente para os aniversariantes do mês;•	Nas sextas-feiras o nosso o expediente se encerra as 16h #Sextou;•	Vestimenta Casual (todos os dias): aqui você pode ser quem é! ;)•	Disponibilizamos frutas no escritório;•	Por aqui gostamos de celebrar os bons momentos, por isso temos Happy Hour com a galera no escritório 1x no mês com chopp e comidinhas;•	Auxílio Home Office de R$ 200,00 – Disponibilizado uma única vez;•	Auxílio Internet de R$ 100,00 – Disponibilizado mensalmente;•	Somos uma empresa cidadã! Licença maternidade e paternidade estendida para nossos Reclovers: 6 meses para mamães e 20 dias para os papais;•	Auxílio-creche para as mamães;•	Fique OK – Programa de apoio social para orientações através de profissionais como: psicólogo, assistente social, advogado, nutricionista, consultor financeiro, consultor pet, fisioterapeuta e personal trainer;•	Estamos trabalhando em modelo híbrido e nosso escritório fica no coração de São Paulo, a Avenida Paulista!Quer ser parte do nosso time? Vem, #todosjuntos fazemos a diferença!</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Vagas.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.vagas.com.br/vagas/v2600553/jovem-aprendiz-ti</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Publicada em 11/01/2024</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>2024-02-11</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-02-03</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Cientista de Dados</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Auxiliar/Operacional</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Jovem Aprendiz - TI</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Worley</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>SP</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Não informado</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
         <is>
           <t>Regime CLT</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr">
         <is>
           <t>['Assistência médica', 'Assistência odontológica', 'Convênio com empresas parceiras', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>v2600553</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>Descrição
 Descrição: Não somos apenas engenheiros. Somos uma equipe global de cientistas de dados, consultores, trabalhadores da construção e inovadores, todos trabalhando para criar um amanhã melhor.Seja qual for a sua ambição, há um caminho para você aqui! #WeAreWorleyEstamos buscando uma pessoa Aprendiz para dar suporte na área de Tecnologia da Informação em projetos da Worley.Outros requisitos: 
@@ -803,85 +962,82 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Vagas.com</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>https://www.vagas.com.br/vagas/v2579647/estagio-em-engenharia-mecanica-tubulacao</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
         <is>
           <t>Publicada em 01/11/2023</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>2024-02-12</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-02-03</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024-02-07</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>Cientista de Dados</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Estágio</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Estágio em Engenharia Mecânica/Tubulação</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Worley</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Belo Horizonte</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>MG</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Não informado</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
         <is>
           <t>Estágio</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
         <is>
           <t>['Assistência médica', 'Assistência odontológica', 'Bolsa auxílio', 'Convênio com empresas parceiras', 'Desconto em produtos', 'Seguro de vida', 'Vale-refeição', 'Vale-transporte']</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="R7" t="inlineStr">
         <is>
           <t>v2579647</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>Descrição
 Descrição: Estamos buscando pessoas estagiárias para fazer parte do time de MMM em Belo Horizonte.Atividades:

</xml_diff>